<commit_message>
[GEN MAIN]BOM에 SMT/DIP type 구별
</commit_message>
<xml_diff>
--- a/2_LF_Generator_Main/1_Schematic/Plasma_LF_Generator_Main_V2.0_BOM.xlsx
+++ b/2_LF_Generator_Main/1_Schematic/Plasma_LF_Generator_Main_V2.0_BOM.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171211_Femto_LF Gen\0_GitHub_Data_LF\2_LF_Generator_Main\1_Schematic\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12060"/>
   </bookViews>
@@ -17,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">LF_Generator_Main_V2.0_SCH!$B$5:$L$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="293">
   <si>
     <t>No</t>
   </si>
@@ -60,9 +55,6 @@
     <t>P_size</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>PCX2-335MB474</t>
   </si>
   <si>
@@ -684,9 +676,6 @@
     <t>6.2x5.0</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>HOLE4.0MM</t>
   </si>
   <si>
@@ -901,6 +890,14 @@
   </si>
   <si>
     <t>ICBanQ</t>
+  </si>
+  <si>
+    <t>DIP</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMT</t>
+    <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -908,7 +905,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -1729,7 +1726,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
@@ -1786,9 +1783,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="18" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1806,6 +1800,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -2124,7 +2121,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2134,13 +2131,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.375" customWidth="1"/>
+    <col min="1" max="1" width="8.375" style="4" customWidth="1"/>
     <col min="2" max="2" width="6.75" customWidth="1"/>
     <col min="3" max="3" width="22.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.125" style="4" customWidth="1"/>
@@ -2156,110 +2153,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8"/>
       <c r="B1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>291</v>
+      </c>
+      <c r="H3">
+        <f>SUMIF(A6:A50,G3,H6:H50)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>292</v>
+      </c>
+      <c r="H4">
+        <f>SUMIF(A6:A50,G4,H6:H50)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="18" t="s">
         <v>283</v>
       </c>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="4" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="19" t="s">
+      <c r="N5" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="O5" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="P5" s="21" t="s">
         <v>286</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="Q5" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="P5" s="22" t="s">
+      <c r="R5" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="Q5" s="22" t="s">
+      <c r="S5" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="T5" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="S5" s="22" t="s">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>291</v>
-      </c>
-      <c r="T5" s="23" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="H6" s="2">
         <v>2</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="L6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M6" s="2">
         <v>350</v>
@@ -2273,41 +2288,41 @@
       <c r="T6" s="15"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
+      <c r="A7" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B7" s="10">
         <v>2</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>23</v>
       </c>
       <c r="H7" s="11">
         <v>2</v>
       </c>
       <c r="I7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="L7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M7" s="11">
         <v>60</v>
@@ -2321,41 +2336,41 @@
       <c r="T7" s="6"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>12</v>
+      <c r="A8" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B8" s="10">
         <v>3</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="F8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="H8" s="11">
         <v>1</v>
       </c>
       <c r="I8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="L8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M8" s="11">
         <v>100</v>
@@ -2369,41 +2384,41 @@
       <c r="T8" s="6"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
+      <c r="A9" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B9" s="10">
         <v>4</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>37</v>
       </c>
       <c r="H9" s="11">
         <v>2</v>
       </c>
       <c r="I9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="L9" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M9" s="11">
         <v>2500</v>
@@ -2417,41 +2432,41 @@
       <c r="T9" s="6"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>12</v>
+      <c r="A10" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B10" s="10">
         <v>5</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>44</v>
       </c>
       <c r="H10" s="11">
         <v>2</v>
       </c>
       <c r="I10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>46</v>
-      </c>
       <c r="K10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M10" s="11">
         <v>2500</v>
@@ -2465,41 +2480,41 @@
       <c r="T10" s="6"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>12</v>
+      <c r="A11" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B11" s="10">
         <v>6</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="H11" s="11">
         <v>4</v>
       </c>
       <c r="I11" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="J11" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>53</v>
-      </c>
       <c r="L11" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M11" s="11">
         <v>210</v>
@@ -2513,41 +2528,41 @@
       <c r="T11" s="6"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>12</v>
+      <c r="A12" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B12" s="10">
         <v>7</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="H12" s="11">
         <v>2</v>
       </c>
       <c r="I12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="K12" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="L12" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M12" s="11">
         <v>40</v>
@@ -2561,41 +2576,41 @@
       <c r="T12" s="6"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>12</v>
+      <c r="A13" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B13" s="10">
         <v>8</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="H13" s="11">
         <v>2</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M13" s="11">
         <v>210</v>
@@ -2609,41 +2624,41 @@
       <c r="T13" s="6"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
+      <c r="A14" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B14" s="10">
         <v>9</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>69</v>
       </c>
       <c r="H14" s="11">
         <v>7</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M14" s="11">
         <v>210</v>
@@ -2657,41 +2672,41 @@
       <c r="T14" s="6"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>12</v>
+      <c r="A15" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B15" s="10">
         <v>10</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="F15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="H15" s="11">
         <v>2</v>
       </c>
       <c r="I15" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="K15" s="11" t="s">
+      <c r="L15" s="11" t="s">
         <v>76</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="M15" s="11">
         <v>1210</v>
@@ -2705,41 +2720,41 @@
       <c r="T15" s="6"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>12</v>
+      <c r="A16" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B16" s="10">
         <v>11</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>81</v>
       </c>
       <c r="H16" s="11">
         <v>2</v>
       </c>
       <c r="I16" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>83</v>
-      </c>
       <c r="L16" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M16" s="11">
         <v>100</v>
@@ -2753,41 +2768,41 @@
       <c r="T16" s="6"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>12</v>
+      <c r="A17" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B17" s="10">
         <v>12</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D17" s="14">
         <v>330</v>
       </c>
       <c r="E17" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>87</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>88</v>
       </c>
       <c r="H17" s="11">
         <v>2</v>
       </c>
       <c r="I17" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="J17" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>90</v>
-      </c>
       <c r="L17" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M17" s="11">
         <v>10</v>
@@ -2801,41 +2816,41 @@
       <c r="T17" s="6"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>12</v>
+      <c r="A18" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B18" s="10">
         <v>13</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="F18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>92</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>93</v>
       </c>
       <c r="H18" s="11">
         <v>3</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M18" s="11">
         <v>10</v>
@@ -2849,41 +2864,41 @@
       <c r="T18" s="6"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>12</v>
+      <c r="A19" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B19" s="10">
         <v>14</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="F19" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>97</v>
       </c>
       <c r="H19" s="11">
         <v>2</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M19" s="11">
         <v>10</v>
@@ -2897,41 +2912,41 @@
       <c r="T19" s="6"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>12</v>
+      <c r="A20" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B20" s="10">
         <v>15</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="E20" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="H20" s="11">
         <v>2</v>
       </c>
       <c r="I20" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="K20" s="11" t="s">
+      <c r="L20" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="M20" s="11">
         <v>10</v>
@@ -2945,41 +2960,41 @@
       <c r="T20" s="6"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>12</v>
+      <c r="A21" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B21" s="10">
         <v>16</v>
       </c>
       <c r="C21" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="E21" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="11" t="s">
         <v>108</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>109</v>
       </c>
       <c r="H21" s="11">
         <v>3</v>
       </c>
       <c r="I21" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="K21" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="J21" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="K21" s="11" t="s">
+      <c r="L21" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="L21" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="M21" s="11">
         <v>10</v>
@@ -2993,41 +3008,41 @@
       <c r="T21" s="6"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>12</v>
+      <c r="A22" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B22" s="10">
         <v>17</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="E22" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="H22" s="11">
         <v>6</v>
       </c>
       <c r="I22" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="K22" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>119</v>
-      </c>
       <c r="L22" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M22" s="11">
         <v>10</v>
@@ -3041,41 +3056,41 @@
       <c r="T22" s="6"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>12</v>
+      <c r="A23" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B23" s="10">
         <v>18</v>
       </c>
       <c r="C23" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="F23" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="H23" s="11">
         <v>2</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J23" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L23" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M23" s="11">
         <v>10</v>
@@ -3089,41 +3104,41 @@
       <c r="T23" s="6"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>12</v>
+      <c r="A24" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B24" s="10">
         <v>19</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="F24" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>126</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>127</v>
       </c>
       <c r="H24" s="11">
         <v>1</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L24" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M24" s="11">
         <v>10</v>
@@ -3137,41 +3152,41 @@
       <c r="T24" s="6"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>12</v>
+      <c r="A25" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B25" s="10">
         <v>20</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="E25" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>130</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>131</v>
       </c>
       <c r="H25" s="11">
         <v>1</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K25" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="L25" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="L25" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="M25" s="11">
         <v>10</v>
@@ -3185,41 +3200,41 @@
       <c r="T25" s="6"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>12</v>
+      <c r="A26" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B26" s="10">
         <v>21</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="E26" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>136</v>
       </c>
       <c r="H26" s="11">
         <v>1</v>
       </c>
       <c r="I26" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="K26" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="J26" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="K26" s="11" t="s">
+      <c r="L26" s="13" t="s">
         <v>138</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
@@ -3231,41 +3246,41 @@
       <c r="T26" s="6"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>12</v>
+      <c r="A27" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B27" s="10">
         <v>22</v>
       </c>
       <c r="C27" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="F27" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>142</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="H27" s="11">
         <v>1</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L27" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M27" s="11">
         <v>10</v>
@@ -3279,41 +3294,41 @@
       <c r="T27" s="6"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>12</v>
+      <c r="A28" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B28" s="10">
         <v>23</v>
       </c>
       <c r="C28" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="E28" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="F28" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G28" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="H28" s="11">
         <v>1</v>
       </c>
       <c r="I28" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="K28" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>150</v>
-      </c>
       <c r="L28" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M28" s="11">
         <v>80</v>
@@ -3327,41 +3342,41 @@
       <c r="T28" s="6"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>12</v>
+      <c r="A29" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B29" s="10">
         <v>24</v>
       </c>
       <c r="C29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="E29" s="11" t="s">
+      <c r="F29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G29" s="11" t="s">
         <v>153</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>154</v>
       </c>
       <c r="H29" s="11">
         <v>1</v>
       </c>
       <c r="I29" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="K29" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="J29" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>156</v>
-      </c>
       <c r="L29" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M29" s="11">
         <v>500</v>
@@ -3375,41 +3390,41 @@
       <c r="T29" s="6"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>12</v>
+      <c r="A30" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B30" s="10">
         <v>25</v>
       </c>
       <c r="C30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="E30" s="11" t="s">
+      <c r="F30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="G30" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="H30" s="11">
         <v>2</v>
       </c>
       <c r="I30" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="K30" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="J30" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="K30" s="11" t="s">
+      <c r="L30" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="L30" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="M30" s="11">
         <v>40</v>
@@ -3423,41 +3438,41 @@
       <c r="T30" s="6"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>12</v>
+      <c r="A31" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B31" s="10">
         <v>26</v>
       </c>
       <c r="C31" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="G31" s="11" t="s">
         <v>165</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>166</v>
       </c>
       <c r="H31" s="11">
         <v>2</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K31" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="L31" s="11" t="s">
         <v>162</v>
-      </c>
-      <c r="L31" s="11" t="s">
-        <v>163</v>
       </c>
       <c r="M31" s="11">
         <v>40</v>
@@ -3471,41 +3486,41 @@
       <c r="T31" s="6"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>12</v>
+      <c r="A32" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B32" s="10">
         <v>27</v>
       </c>
       <c r="C32" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" s="11" t="s">
+      <c r="F32" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="G32" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="H32" s="11">
         <v>1</v>
       </c>
       <c r="I32" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="K32" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="J32" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>172</v>
-      </c>
       <c r="L32" s="11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M32" s="11">
         <v>520</v>
@@ -3519,41 +3534,41 @@
       <c r="T32" s="6"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>12</v>
+      <c r="A33" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B33" s="10">
         <v>28</v>
       </c>
       <c r="C33" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="E33" s="11" t="s">
+      <c r="F33" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G33" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>176</v>
       </c>
       <c r="H33" s="11">
         <v>1</v>
       </c>
       <c r="I33" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="K33" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="J33" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>178</v>
-      </c>
       <c r="L33" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M33" s="11">
         <v>70</v>
@@ -3567,41 +3582,41 @@
       <c r="T33" s="6"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>12</v>
+      <c r="A34" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B34" s="10">
         <v>29</v>
       </c>
       <c r="C34" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>180</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F34" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="G34" s="11" t="s">
-        <v>181</v>
       </c>
       <c r="H34" s="11">
         <v>2</v>
       </c>
       <c r="I34" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="K34" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="J34" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>183</v>
-      </c>
       <c r="L34" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M34" s="11">
         <v>180</v>
@@ -3615,41 +3630,41 @@
       <c r="T34" s="6"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>12</v>
+      <c r="A35" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B35" s="10">
         <v>30</v>
       </c>
       <c r="C35" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>185</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="G35" s="11" t="s">
-        <v>186</v>
       </c>
       <c r="H35" s="11">
         <v>2</v>
       </c>
       <c r="I35" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="K35" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="J35" s="11" t="s">
+      <c r="L35" s="11" t="s">
         <v>184</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="L35" s="11" t="s">
-        <v>185</v>
       </c>
       <c r="M35" s="11">
         <v>200</v>
@@ -3663,41 +3678,41 @@
       <c r="T35" s="6"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>12</v>
+      <c r="A36" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B36" s="10">
         <v>31</v>
       </c>
       <c r="C36" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="E36" s="11" t="s">
+      <c r="F36" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="G36" s="11" t="s">
         <v>190</v>
-      </c>
-      <c r="F36" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="G36" s="11" t="s">
-        <v>191</v>
       </c>
       <c r="H36" s="11">
         <v>2</v>
       </c>
       <c r="I36" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="K36" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="J36" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="K36" s="11" t="s">
-        <v>193</v>
-      </c>
       <c r="L36" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M36" s="11">
         <v>16900</v>
@@ -3711,41 +3726,41 @@
       <c r="T36" s="6"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>12</v>
+      <c r="A37" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B37" s="10">
         <v>32</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="E37" s="11" t="s">
+      <c r="F37" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="G37" s="11" t="s">
         <v>196</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="G37" s="11" t="s">
-        <v>197</v>
       </c>
       <c r="H37" s="11">
         <v>2</v>
       </c>
       <c r="I37" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="K37" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="J37" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>199</v>
-      </c>
       <c r="L37" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M37" s="11">
         <v>3640</v>
@@ -3759,41 +3774,41 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>12</v>
+      <c r="A38" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B38" s="10">
         <v>33</v>
       </c>
       <c r="C38" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="E38" s="11" t="s">
+      <c r="F38" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G38" s="11" t="s">
         <v>202</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>203</v>
       </c>
       <c r="H38" s="11">
         <v>1</v>
       </c>
       <c r="I38" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="K38" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="J38" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="K38" s="11" t="s">
+      <c r="L38" s="11" t="s">
         <v>205</v>
-      </c>
-      <c r="L38" s="11" t="s">
-        <v>206</v>
       </c>
       <c r="M38" s="11">
         <v>5100</v>
@@ -3807,41 +3822,41 @@
       <c r="T38" s="6"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>12</v>
+      <c r="A39" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B39" s="10">
         <v>34</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="E39" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="F39" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="G39" s="11" t="s">
         <v>210</v>
-      </c>
-      <c r="F39" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>211</v>
       </c>
       <c r="H39" s="11">
         <v>1</v>
       </c>
       <c r="I39" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="K39" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="J39" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="K39" s="11" t="s">
-        <v>213</v>
-      </c>
       <c r="L39" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M39" s="11">
         <v>2850</v>
@@ -3855,41 +3870,41 @@
       <c r="T39" s="6"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>12</v>
+      <c r="A40" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B40" s="10">
         <v>35</v>
       </c>
       <c r="C40" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E40" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="E40" s="11" t="s">
+      <c r="F40" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="G40" s="11" t="s">
         <v>216</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>217</v>
       </c>
       <c r="H40" s="11">
         <v>1</v>
       </c>
       <c r="I40" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="J40" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="J40" s="11" t="s">
-        <v>219</v>
-      </c>
       <c r="K40" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L40" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M40" s="11">
         <v>350</v>
@@ -3903,41 +3918,41 @@
       <c r="T40" s="6"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>12</v>
+      <c r="A41" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B41" s="10">
         <v>37</v>
       </c>
       <c r="C41" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="G41" s="11" t="s">
         <v>223</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F41" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>225</v>
       </c>
       <c r="H41" s="11">
         <v>8</v>
       </c>
       <c r="I41" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="J41" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="J41" s="11" t="s">
-        <v>228</v>
-      </c>
       <c r="K41" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="L41" s="11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M41" s="11">
         <v>10</v>
@@ -3951,41 +3966,41 @@
       <c r="T41" s="6"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>12</v>
+      <c r="A42" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B42" s="10">
         <v>38</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="E42" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="F42" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="G42" s="11" t="s">
         <v>230</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="G42" s="11" t="s">
-        <v>232</v>
       </c>
       <c r="H42" s="11">
         <v>1</v>
       </c>
       <c r="I42" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="J42" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="J42" s="11" t="s">
-        <v>235</v>
-      </c>
       <c r="K42" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L42" s="11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M42" s="11">
         <v>250</v>
@@ -3999,41 +4014,41 @@
       <c r="T42" s="6"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>12</v>
+      <c r="A43" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B43" s="10">
         <v>39</v>
       </c>
       <c r="C43" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="F43" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="G43" s="11" t="s">
         <v>237</v>
-      </c>
-      <c r="E43" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="F43" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="G43" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="H43" s="11">
         <v>2</v>
       </c>
       <c r="I43" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="J43" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="J43" s="11" t="s">
-        <v>242</v>
-      </c>
       <c r="K43" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L43" s="11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M43" s="11">
         <v>1200</v>
@@ -4047,41 +4062,41 @@
       <c r="T43" s="6"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>12</v>
+      <c r="A44" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B44" s="10">
         <v>40</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H44" s="11">
         <v>1</v>
       </c>
       <c r="I44" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="J44" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="J44" s="11" t="s">
-        <v>247</v>
-      </c>
       <c r="K44" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M44" s="11">
         <v>120</v>
@@ -4095,41 +4110,41 @@
       <c r="T44" s="6"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>12</v>
+      <c r="A45" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B45" s="10">
         <v>42</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G45" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H45" s="11">
         <v>2</v>
       </c>
       <c r="I45" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="J45" s="11" t="s">
         <v>257</v>
       </c>
-      <c r="J45" s="11" t="s">
-        <v>259</v>
-      </c>
       <c r="K45" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L45" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
@@ -4141,41 +4156,41 @@
       <c r="T45" s="6"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>12</v>
+      <c r="A46" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B46" s="10">
         <v>43</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="G46" s="11" t="s">
         <v>260</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="G46" s="11" t="s">
-        <v>262</v>
       </c>
       <c r="H46" s="11">
         <v>1</v>
       </c>
       <c r="I46" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="J46" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="J46" s="11" t="s">
-        <v>265</v>
-      </c>
       <c r="K46" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L46" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M46" s="11">
         <v>20800</v>
@@ -4189,41 +4204,41 @@
       <c r="T46" s="6"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>12</v>
+      <c r="A47" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="B47" s="10">
         <v>44</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H47" s="11">
         <v>2</v>
       </c>
       <c r="I47" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="J47" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="J47" s="11" t="s">
-        <v>270</v>
-      </c>
       <c r="K47" s="11" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L47" s="11" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M47" s="11">
         <v>480</v>
@@ -4237,41 +4252,41 @@
       <c r="T47" s="6"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>12</v>
+      <c r="A48" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B48" s="10">
         <v>45</v>
       </c>
       <c r="C48" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="E48" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="F48" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="G48" s="11" t="s">
         <v>272</v>
-      </c>
-      <c r="E48" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>274</v>
       </c>
       <c r="H48" s="11">
         <v>1</v>
       </c>
       <c r="I48" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="J48" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="J48" s="11" t="s">
-        <v>277</v>
-      </c>
       <c r="K48" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L48" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="M48" s="11">
         <v>45000</v>
@@ -4285,41 +4300,41 @@
       <c r="T48" s="6"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>12</v>
+      <c r="A49" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B49" s="10">
         <v>46</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H49" s="11">
         <v>1</v>
       </c>
       <c r="I49" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="J49" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="J49" s="11" t="s">
-        <v>282</v>
-      </c>
       <c r="K49" s="11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L49" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M49" s="11">
         <v>500</v>
@@ -4333,41 +4348,41 @@
       <c r="T49" s="6"/>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>220</v>
+      <c r="A50" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="B50" s="10">
         <v>41</v>
       </c>
       <c r="C50" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="E50" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="F50" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="G50" s="11" t="s">
         <v>249</v>
-      </c>
-      <c r="E50" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="G50" s="11" t="s">
-        <v>251</v>
       </c>
       <c r="H50" s="11">
         <v>1</v>
       </c>
       <c r="I50" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="J50" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="J50" s="11" t="s">
-        <v>254</v>
-      </c>
       <c r="K50" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="L50" s="11" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M50" s="11">
         <v>120</v>
@@ -4381,14 +4396,11 @@
       <c r="T50" s="6"/>
     </row>
     <row r="51" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>220</v>
-      </c>
       <c r="B51" s="5">
         <v>36</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="9"/>
@@ -4398,14 +4410,14 @@
         <v>6</v>
       </c>
       <c r="I51" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J51" s="9">
         <v>0</v>
       </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
@@ -4416,9 +4428,16 @@
       <c r="S51" s="9"/>
       <c r="T51" s="16"/>
     </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H52">
+        <f>SUM(H6:H50)</f>
+        <v>91</v>
+      </c>
+    </row>
     <row r="53" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="8"/>
       <c r="B53" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D53" s="8"/>
     </row>

</xml_diff>